<commit_message>
Fix payload mapping for rbi_email and tiu_email
</commit_message>
<xml_diff>
--- a/template/Gudipati_Phani_Babu_Timesheet_Week_Ending_08152025.xlsx
+++ b/template/Gudipati_Phani_Babu_Timesheet_Week_Ending_08152025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phani/Downloads/timesheet_tool_starter/backend/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E01AAFC-7491-7D45-AB97-A550DFF0F514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C60860-87AE-354A-B302-0EFD57A0DA2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="15880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>EMPLOYEE DETAILS:</t>
   </si>
@@ -145,6 +145,12 @@
   </si>
   <si>
     <t>08-13-2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                          RBI Email :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                   TIU Email :</t>
   </si>
 </sst>
 </file>
@@ -156,9 +162,16 @@
     <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
     <numFmt numFmtId="166" formatCode="[$-409]h:mm\ AM/PM;@"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -321,32 +334,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="39" fontId="6" fillId="0" borderId="0">
+    <xf numFmtId="39" fontId="7" fillId="0" borderId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="4" fontId="7" fillId="0" borderId="0">
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
@@ -365,76 +378,82 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="39" fontId="9" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="39" fontId="10" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="39" fontId="8" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="10" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="39" fontId="9" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="8" applyFill="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="8" applyNumberFormat="1" applyFill="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="11" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="2" fillId="3" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="14" fontId="9" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="8" applyFill="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="8" applyNumberFormat="1" applyFill="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="3" borderId="3" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -846,7 +865,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -899,7 +918,9 @@
       <c r="C4" s="20"/>
       <c r="D4" s="8"/>
       <c r="E4" s="12"/>
-      <c r="F4" s="9"/>
+      <c r="F4" s="31" t="s">
+        <v>34</v>
+      </c>
       <c r="G4" s="23" t="s">
         <v>3</v>
       </c>
@@ -911,7 +932,9 @@
       <c r="C5" s="4"/>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
-      <c r="F5" s="10"/>
+      <c r="F5" s="32" t="s">
+        <v>35</v>
+      </c>
       <c r="G5" s="24" t="s">
         <v>4</v>
       </c>
@@ -919,14 +942,14 @@
     </row>
     <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
       <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -991,76 +1014,76 @@
     </row>
     <row r="11" spans="1:8" s="1" customFormat="1" ht="40.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="29" t="s">
+      <c r="E11" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="F11" s="29" t="s">
+      <c r="F11" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="29" t="s">
+      <c r="G11" s="27" t="s">
         <v>11</v>
       </c>
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="30">
+      <c r="C12" s="28">
         <v>8</v>
       </c>
-      <c r="D12" s="30">
+      <c r="D12" s="28">
         <v>8</v>
       </c>
-      <c r="E12" s="30">
+      <c r="E12" s="28">
         <v>8</v>
       </c>
-      <c r="F12" s="30">
+      <c r="F12" s="28">
         <v>8</v>
       </c>
-      <c r="G12" s="30">
+      <c r="G12" s="28">
         <v>8</v>
       </c>
       <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
       <c r="H13" s="18"/>
     </row>
     <row r="14" spans="1:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
       <c r="H14" s="18"/>
     </row>
     <row r="15" spans="1:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
       <c r="H15" s="18"/>
     </row>
     <row r="16" spans="1:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>